<commit_message>
update schedule for borey
</commit_message>
<xml_diff>
--- a/app/storage/packages/loan/Repayment Schedule Borey.xlsx
+++ b/app/storage/packages/loan/Repayment Schedule Borey.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>កាលវិភាគសងប្រាក់</t>
   </si>
@@ -258,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -290,6 +290,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -299,25 +315,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -640,48 +649,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
@@ -689,72 +698,72 @@
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="13"/>
+      <c r="F5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15" t="s">
+      <c r="E6" s="13"/>
+      <c r="F6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15" t="s">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="15"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="14"/>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="15"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="17" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -827,64 +836,96 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="20" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="21">
+        <f>SUM(C11:C12)</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="22">
+        <f>SUM(D11:D12)</f>
+        <v>10000000</v>
+      </c>
+      <c r="E13" s="22">
+        <f>SUM(E11:E12)</f>
+        <v>2000</v>
+      </c>
+      <c r="F13" s="22">
+        <f>SUM(F11:F12)</f>
+        <v>10002000</v>
+      </c>
+      <c r="G13" s="22"/>
+    </row>
+    <row r="14" spans="1:7" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="19"/>
-    </row>
-    <row r="14" spans="1:7" s="20" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="19"/>
-    </row>
-    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F16" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="F17" s="6" t="s">
+    <row r="17" spans="2:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="F18" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+    <row r="19" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+    <row r="20" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A2:G2"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="A9:C9"/>
@@ -896,15 +937,6 @@
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:G9"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A2:G2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
update schedule for borey 2
</commit_message>
<xml_diff>
--- a/app/storage/packages/loan/Repayment Schedule Borey.xlsx
+++ b/app/storage/packages/loan/Repayment Schedule Borey.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" refMode="R1C1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -294,38 +294,38 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,7 +634,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -660,15 +660,15 @@
       <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -693,77 +693,77 @@
       <c r="G4" s="19"/>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="13" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13" t="s">
+      <c r="E5" s="21"/>
+      <c r="F5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="13"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13" t="s">
+      <c r="E6" s="21"/>
+      <c r="F6" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="13"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13" t="s">
+      <c r="E7" s="21"/>
+      <c r="F7" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="13"/>
+      <c r="G7" s="21"/>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="13" t="s">
+      <c r="E8" s="20"/>
+      <c r="F8" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="13"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="15" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -837,27 +837,27 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="23" t="s">
+      <c r="A13" s="13"/>
+      <c r="B13" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="13">
         <f>SUM(C11:C12)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="14">
         <f>SUM(D11:D12)</f>
         <v>10000000</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="14">
         <f>SUM(E11:E12)</f>
         <v>2000</v>
       </c>
-      <c r="F13" s="22">
-        <f>SUM(F11:F12)</f>
+      <c r="F13" s="14">
+        <f>D13+E13</f>
         <v>10002000</v>
       </c>
-      <c r="G13" s="22"/>
+      <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
@@ -917,6 +917,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:G9"/>
     <mergeCell ref="A14:F14"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A1:G1"/>
@@ -933,10 +937,6 @@
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:G9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>